<commit_message>
EPBDS-14277 Output Model Description
</commit_message>
<xml_diff>
--- a/ITEST/itest.smoke/openl-repository/deployments/openapi/openapi/Bank Rating.xlsx
+++ b/ITEST/itest.smoke/openl-repository/deployments/openapi/openapi/Bank Rating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\ITEST\itest.smoke\openl-repository\deployments\openapi\openapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2439A71-66AB-47BD-B6A5-7555143586ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E52322-5B1F-4A53-B009-8100844D1FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9130" yWindow="900" windowWidth="20490" windowHeight="16630" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="850" yWindow="1240" windowWidth="20990" windowHeight="15360" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="18" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="161">
   <si>
     <t>R3</t>
   </si>
@@ -670,6 +670,48 @@
   </si>
   <si>
     <t>3.1023, 2, -1.0303003</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult myCalc(Integer a)</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Values1</t>
+  </si>
+  <si>
+    <t>// Values1</t>
+  </si>
+  <si>
+    <t>Values2</t>
+  </si>
+  <si>
+    <t>// Values2</t>
+  </si>
+  <si>
+    <t>RETURN1</t>
+  </si>
+  <si>
+    <t>= new Integer(7)</t>
+  </si>
+  <si>
+    <t>BComment1</t>
+  </si>
+  <si>
+    <t>= new Double(5)</t>
+  </si>
+  <si>
+    <t>RETURN3</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>AComment1</t>
+  </si>
+  <si>
+    <t>RETURN2</t>
   </si>
 </sst>
 </file>
@@ -756,7 +798,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1023,12 +1065,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1063,6 +1123,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Heading 1" xfId="1" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
@@ -1451,7 +1519,7 @@
   </sheetPr>
   <dimension ref="A2:AMJ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -1938,10 +2006,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0504C1-C546-4B06-829C-4444E3B89613}">
-  <dimension ref="C5:E27"/>
+  <dimension ref="C5:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:E24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.4"/>
@@ -2063,8 +2131,154 @@
       </c>
       <c r="E27" s="22"/>
     </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C33" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C34" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="27"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C35" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="G35" s="28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C36" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C37" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="G37" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C41" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="25"/>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C42" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42" t="s">
+        <v>158</v>
+      </c>
+      <c r="G42" s="27"/>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C43" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="F43" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="G43" s="28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C44" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="F44" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="G44" s="29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.4">
+      <c r="C45" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="G45" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C41:G41"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>

</xml_diff>